<commit_message>
Natmi following Dr Hou advice
</commit_message>
<xml_diff>
--- a/natmiOut/OldD0/LR-pairs_lrc2p/Ace-Bdkrb2.xlsx
+++ b/natmiOut/OldD0/LR-pairs_lrc2p/Ace-Bdkrb2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="25">
   <si>
     <t>Sending cluster</t>
   </si>
@@ -446,7 +446,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:T10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -525,60 +525,60 @@
         <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2">
-        <v>16.2369699081652</v>
+        <v>32.50384966666667</v>
       </c>
       <c r="H2">
-        <v>16.2369699081652</v>
+        <v>97.511549</v>
       </c>
       <c r="I2">
-        <v>0.06208864493580833</v>
+        <v>0.1162664629566559</v>
       </c>
       <c r="J2">
-        <v>0.06208864493580833</v>
+        <v>0.116266462956656</v>
       </c>
       <c r="K2">
         <v>1</v>
       </c>
       <c r="L2">
-        <v>1</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="M2">
-        <v>0.796511238273539</v>
+        <v>0.3006476666666667</v>
       </c>
       <c r="N2">
-        <v>0.796511238273539</v>
+        <v>0.9019430000000001</v>
       </c>
       <c r="O2">
-        <v>1</v>
+        <v>0.2555551336960822</v>
       </c>
       <c r="P2">
-        <v>1</v>
+        <v>0.2555551336960821</v>
       </c>
       <c r="Q2">
-        <v>12.93292900736285</v>
+        <v>9.772206559967445</v>
       </c>
       <c r="R2">
-        <v>12.93292900736285</v>
+        <v>87.94985903970701</v>
       </c>
       <c r="S2">
-        <v>0.06208864493580833</v>
+        <v>0.0297124914852588</v>
       </c>
       <c r="T2">
-        <v>0.06208864493580833</v>
+        <v>0.0297124914852588</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
         <v>23</v>
@@ -590,57 +590,57 @@
         <v>21</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3">
-        <v>244.145785680615</v>
+        <v>32.50384966666667</v>
       </c>
       <c r="H3">
-        <v>244.145785680615</v>
+        <v>97.511549</v>
       </c>
       <c r="I3">
-        <v>0.9335905089086055</v>
+        <v>0.1162664629566559</v>
       </c>
       <c r="J3">
-        <v>0.9335905089086055</v>
+        <v>0.116266462956656</v>
       </c>
       <c r="K3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L3">
         <v>1</v>
       </c>
       <c r="M3">
-        <v>0.796511238273539</v>
+        <v>0.8000553333333333</v>
       </c>
       <c r="N3">
-        <v>0.796511238273539</v>
+        <v>2.400166</v>
       </c>
       <c r="O3">
-        <v>1</v>
+        <v>0.6800593197383766</v>
       </c>
       <c r="P3">
-        <v>1</v>
+        <v>0.6800593197383766</v>
       </c>
       <c r="Q3">
-        <v>194.4648620717327</v>
+        <v>26.00487827968156</v>
       </c>
       <c r="R3">
-        <v>194.4648620717327</v>
+        <v>234.043904517134</v>
       </c>
       <c r="S3">
-        <v>0.9335905089086055</v>
+        <v>0.07906809170669062</v>
       </c>
       <c r="T3">
-        <v>0.9335905089086055</v>
+        <v>0.07906809170669062</v>
       </c>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
         <v>23</v>
@@ -649,55 +649,427 @@
         <v>24</v>
       </c>
       <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>32.50384966666667</v>
+      </c>
+      <c r="H4">
+        <v>97.511549</v>
+      </c>
+      <c r="I4">
+        <v>0.1162664629566559</v>
+      </c>
+      <c r="J4">
+        <v>0.116266462956656</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="M4">
+        <v>0.07574633333333333</v>
+      </c>
+      <c r="N4">
+        <v>0.227239</v>
+      </c>
+      <c r="O4">
+        <v>0.06438554656554128</v>
+      </c>
+      <c r="P4">
+        <v>0.06438554656554128</v>
+      </c>
+      <c r="Q4">
+        <v>2.462047431467889</v>
+      </c>
+      <c r="R4">
+        <v>22.158426883211</v>
+      </c>
+      <c r="S4">
+        <v>0.007485879764706552</v>
+      </c>
+      <c r="T4">
+        <v>0.007485879764706553</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
+      <c r="A5" t="s">
         <v>21</v>
       </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>1.12995619534941</v>
-      </c>
-      <c r="H4">
-        <v>1.12995619534941</v>
-      </c>
-      <c r="I4">
-        <v>0.004320846155586321</v>
-      </c>
-      <c r="J4">
-        <v>0.004320846155586321</v>
-      </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4">
-        <v>1</v>
-      </c>
-      <c r="M4">
-        <v>0.796511238273539</v>
-      </c>
-      <c r="N4">
-        <v>0.796511238273539</v>
-      </c>
-      <c r="O4">
-        <v>1</v>
-      </c>
-      <c r="P4">
-        <v>1</v>
-      </c>
-      <c r="Q4">
-        <v>0.9000228083526154</v>
-      </c>
-      <c r="R4">
-        <v>0.9000228083526154</v>
-      </c>
-      <c r="S4">
-        <v>0.004320846155586321</v>
-      </c>
-      <c r="T4">
-        <v>0.004320846155586321</v>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>245.8810833333334</v>
+      </c>
+      <c r="H5">
+        <v>737.6432500000001</v>
+      </c>
+      <c r="I5">
+        <v>0.8795180927887045</v>
+      </c>
+      <c r="J5">
+        <v>0.8795180927887046</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="M5">
+        <v>0.3006476666666667</v>
+      </c>
+      <c r="N5">
+        <v>0.9019430000000001</v>
+      </c>
+      <c r="O5">
+        <v>0.2555551336960822</v>
+      </c>
+      <c r="P5">
+        <v>0.2555551336960821</v>
+      </c>
+      <c r="Q5">
+        <v>73.9235739816389</v>
+      </c>
+      <c r="R5">
+        <v>665.3121658347501</v>
+      </c>
+      <c r="S5">
+        <v>0.2247653637907406</v>
+      </c>
+      <c r="T5">
+        <v>0.2247653637907406</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>245.8810833333334</v>
+      </c>
+      <c r="H6">
+        <v>737.6432500000001</v>
+      </c>
+      <c r="I6">
+        <v>0.8795180927887045</v>
+      </c>
+      <c r="J6">
+        <v>0.8795180927887046</v>
+      </c>
+      <c r="K6">
+        <v>3</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>0.8000553333333333</v>
+      </c>
+      <c r="N6">
+        <v>2.400166</v>
+      </c>
+      <c r="O6">
+        <v>0.6800593197383766</v>
+      </c>
+      <c r="P6">
+        <v>0.6800593197383766</v>
+      </c>
+      <c r="Q6">
+        <v>196.7184720866111</v>
+      </c>
+      <c r="R6">
+        <v>1770.4662487795</v>
+      </c>
+      <c r="S6">
+        <v>0.5981244758794808</v>
+      </c>
+      <c r="T6">
+        <v>0.5981244758794809</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>245.8810833333334</v>
+      </c>
+      <c r="H7">
+        <v>737.6432500000001</v>
+      </c>
+      <c r="I7">
+        <v>0.8795180927887045</v>
+      </c>
+      <c r="J7">
+        <v>0.8795180927887046</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="M7">
+        <v>0.07574633333333333</v>
+      </c>
+      <c r="N7">
+        <v>0.227239</v>
+      </c>
+      <c r="O7">
+        <v>0.06438554656554128</v>
+      </c>
+      <c r="P7">
+        <v>0.06438554656554128</v>
+      </c>
+      <c r="Q7">
+        <v>18.62459049852778</v>
+      </c>
+      <c r="R7">
+        <v>167.62131448675</v>
+      </c>
+      <c r="S7">
+        <v>0.05662825311848319</v>
+      </c>
+      <c r="T7">
+        <v>0.0566282531184832</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1.178484</v>
+      </c>
+      <c r="H8">
+        <v>3.535452</v>
+      </c>
+      <c r="I8">
+        <v>0.004215444254639368</v>
+      </c>
+      <c r="J8">
+        <v>0.004215444254639368</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="M8">
+        <v>0.3006476666666667</v>
+      </c>
+      <c r="N8">
+        <v>0.9019430000000001</v>
+      </c>
+      <c r="O8">
+        <v>0.2555551336960822</v>
+      </c>
+      <c r="P8">
+        <v>0.2555551336960821</v>
+      </c>
+      <c r="Q8">
+        <v>0.3543084648040001</v>
+      </c>
+      <c r="R8">
+        <v>3.188776183236</v>
+      </c>
+      <c r="S8">
+        <v>0.001077278420082745</v>
+      </c>
+      <c r="T8">
+        <v>0.001077278420082745</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1.178484</v>
+      </c>
+      <c r="H9">
+        <v>3.535452</v>
+      </c>
+      <c r="I9">
+        <v>0.004215444254639368</v>
+      </c>
+      <c r="J9">
+        <v>0.004215444254639368</v>
+      </c>
+      <c r="K9">
+        <v>3</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>0.8000553333333333</v>
+      </c>
+      <c r="N9">
+        <v>2.400166</v>
+      </c>
+      <c r="O9">
+        <v>0.6800593197383766</v>
+      </c>
+      <c r="P9">
+        <v>0.6800593197383766</v>
+      </c>
+      <c r="Q9">
+        <v>0.9428524094480001</v>
+      </c>
+      <c r="R9">
+        <v>8.485671685032001</v>
+      </c>
+      <c r="S9">
+        <v>0.002866752152205097</v>
+      </c>
+      <c r="T9">
+        <v>0.002866752152205097</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1.178484</v>
+      </c>
+      <c r="H10">
+        <v>3.535452</v>
+      </c>
+      <c r="I10">
+        <v>0.004215444254639368</v>
+      </c>
+      <c r="J10">
+        <v>0.004215444254639368</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="M10">
+        <v>0.07574633333333333</v>
+      </c>
+      <c r="N10">
+        <v>0.227239</v>
+      </c>
+      <c r="O10">
+        <v>0.06438554656554128</v>
+      </c>
+      <c r="P10">
+        <v>0.06438554656554128</v>
+      </c>
+      <c r="Q10">
+        <v>0.089265841892</v>
+      </c>
+      <c r="R10">
+        <v>0.803392577028</v>
+      </c>
+      <c r="S10">
+        <v>0.0002714136823515265</v>
+      </c>
+      <c r="T10">
+        <v>0.0002714136823515265</v>
       </c>
     </row>
   </sheetData>

</xml_diff>